<commit_message>
Inclusao custos de transporte no orçamento
</commit_message>
<xml_diff>
--- a/PastaDocsAdministativos/Orcamento.xlsx
+++ b/PastaDocsAdministativos/Orcamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\logonrmlocal\Downloads\GIT-exercicio\3SIPG\PastaDocsAdministativos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741925AC-8E56-4412-B2CE-C7D500EAE3CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E49152F5-40EC-4322-8735-AFE2F354A9EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>PREVISÃO ORÇAMENTÁRIA - PROJETO EXEMPLO</t>
   </si>
@@ -48,10 +48,16 @@
     <t>R$ 320,00</t>
   </si>
   <si>
-    <t>Refeiçoes</t>
-  </si>
-  <si>
     <t>R$147.200</t>
+  </si>
+  <si>
+    <t>TRANSPORTE</t>
+  </si>
+  <si>
+    <t>REFEICOES</t>
+  </si>
+  <si>
+    <t>R$ 49.780</t>
   </si>
 </sst>
 </file>
@@ -369,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,10 +418,18 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>